<commit_message>
update from other account
</commit_message>
<xml_diff>
--- a/Apartment Search.xlsx
+++ b/Apartment Search.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Home</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>adding a line to test</t>
+  </si>
+  <si>
+    <t>anotheradd</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A2:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -603,6 +606,9 @@
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>31</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>